<commit_message>
adding manager and chaging color for buttons
</commit_message>
<xml_diff>
--- a/public/files/appointment-info.xlsx
+++ b/public/files/appointment-info.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Programare</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>2021-05-18 10:00</t>
+  </si>
+  <si>
+    <t>2021-05-24 13:00</t>
+  </si>
+  <si>
+    <t>2021-05-25 12:30</t>
+  </si>
+  <si>
+    <t>Giuredea Manuela-Ioana</t>
+  </si>
+  <si>
+    <t>Pedichiura cu oja semipermanenta</t>
   </si>
 </sst>
 </file>
@@ -398,7 +410,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +518,40 @@
       </c>
       <c r="E6">
         <v>45.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>